<commit_message>
Programação da suavização de Laplace terminada. Nesse commit estamos adicionando ao código a previsão para a tabela teste e a porcentagem de discrepância entre ela e o real feito a mão
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc3228dbb7e0c340/Desktop/PYTHON/CDados/Trabalho 1/22-2a-cd-p1-grupo_henriquefb3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{435CC18E-52FF-4E66-9F9B-865A176B74D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCECF237-D3FE-4AF5-8D14-70155D9EED14}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{435CC18E-52FF-4E66-9F9B-865A176B74D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA62B8A2-705E-468C-90C1-6CBD90D3168E}"/>
   <bookViews>
     <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13444,7 +13444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>